<commit_message>
Added and question on tuition
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camara\Documents\Singapore workshop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camara\Documents\Singapore workshop\WHO_VA_2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t xml:space="preserve">type </t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t xml:space="preserve">constraint message </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tutorials </t>
+  </si>
+  <si>
+    <t xml:space="preserve">which class did you attaend </t>
   </si>
 </sst>
 </file>
@@ -177,11 +183,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,6 +610,17 @@
       </c>
       <c r="H7" s="3" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>